<commit_message>
Yearly Update to the trash bin
</commit_message>
<xml_diff>
--- a/IMMC/Coop/DataOut.xlsx
+++ b/IMMC/Coop/DataOut.xlsx
@@ -1507,11 +1507,6 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1526,11 +1521,6 @@
       <c r="D3" t="n">
         <v>25</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1545,11 +1535,6 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1564,11 +1549,6 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1583,11 +1563,6 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1602,11 +1577,6 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1621,11 +1591,6 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1640,11 +1605,6 @@
       <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1659,11 +1619,6 @@
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1678,11 +1633,6 @@
       <c r="D11" t="n">
         <v>90</v>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1697,11 +1647,6 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1716,11 +1661,6 @@
       <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1735,11 +1675,6 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1754,11 +1689,6 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1773,11 +1703,6 @@
       <c r="D16" t="n">
         <v>15</v>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1792,11 +1717,6 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1811,11 +1731,6 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1830,11 +1745,6 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1849,11 +1759,6 @@
       <c r="D20" t="n">
         <v>0</v>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1868,11 +1773,6 @@
       <c r="D21" t="n">
         <v>15</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1887,11 +1787,6 @@
       <c r="D22" t="n">
         <v>0</v>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1906,11 +1801,6 @@
       <c r="D23" t="n">
         <v>95</v>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1925,11 +1815,6 @@
       <c r="D24" t="n">
         <v>0</v>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1944,11 +1829,6 @@
       <c r="D25" t="n">
         <v>340</v>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1963,11 +1843,6 @@
       <c r="D26" t="n">
         <v>220</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1982,11 +1857,6 @@
       <c r="D27" t="n">
         <v>0</v>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2001,11 +1871,6 @@
       <c r="D28" t="n">
         <v>0</v>
       </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2020,11 +1885,6 @@
       <c r="D29" t="n">
         <v>50</v>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2039,11 +1899,6 @@
       <c r="D30" t="n">
         <v>100</v>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2058,19 +1913,11 @@
       <c r="D31" t="n">
         <v>25</v>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
         <v>982</v>
       </c>
@@ -2080,19 +1927,11 @@
       <c r="G32" t="n">
         <v>975</v>
       </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
         <v>1.111111111111124</v>
       </c>
@@ -4396,6 +4235,13 @@
       <c r="F2" t="n">
         <v>45</v>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -4416,6 +4262,13 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -4436,6 +4289,13 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -4456,6 +4316,13 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -4476,6 +4343,13 @@
       <c r="F6" t="n">
         <v>0</v>
       </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -4496,6 +4370,13 @@
       <c r="F7" t="n">
         <v>200</v>
       </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -4516,6 +4397,13 @@
       <c r="F8" t="n">
         <v>0</v>
       </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -4536,6 +4424,13 @@
       <c r="F9" t="n">
         <v>0</v>
       </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -4556,6 +4451,13 @@
       <c r="F10" t="n">
         <v>1</v>
       </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -4576,6 +4478,13 @@
       <c r="F11" t="n">
         <v>0</v>
       </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -4596,6 +4505,13 @@
       <c r="F12" t="n">
         <v>0</v>
       </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -4616,6 +4532,13 @@
       <c r="F13" t="n">
         <v>0</v>
       </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -4636,6 +4559,13 @@
       <c r="F14" t="n">
         <v>0</v>
       </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -4656,6 +4586,13 @@
       <c r="F15" t="n">
         <v>170</v>
       </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -4676,6 +4613,13 @@
       <c r="F16" t="n">
         <v>0</v>
       </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -4696,6 +4640,13 @@
       <c r="F17" t="n">
         <v>0</v>
       </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -4716,6 +4667,13 @@
       <c r="F18" t="n">
         <v>0</v>
       </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4736,6 +4694,13 @@
       <c r="F19" t="n">
         <v>0</v>
       </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4756,6 +4721,13 @@
       <c r="F20" t="n">
         <v>35</v>
       </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4776,6 +4748,13 @@
       <c r="F21" t="n">
         <v>0</v>
       </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -4796,6 +4775,13 @@
       <c r="F22" t="n">
         <v>0</v>
       </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -4816,6 +4802,13 @@
       <c r="F23" t="n">
         <v>0</v>
       </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -4836,6 +4829,13 @@
       <c r="F24" t="n">
         <v>90</v>
       </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -4856,6 +4856,13 @@
       <c r="F25" t="n">
         <v>0</v>
       </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -4876,6 +4883,13 @@
       <c r="F26" t="n">
         <v>0</v>
       </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -4896,6 +4910,13 @@
       <c r="F27" t="n">
         <v>0</v>
       </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -4916,6 +4937,13 @@
       <c r="F28" t="n">
         <v>0</v>
       </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -4936,6 +4964,13 @@
       <c r="F29" t="n">
         <v>0</v>
       </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -4956,6 +4991,13 @@
       <c r="F30" t="n">
         <v>120</v>
       </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -4976,11 +5018,23 @@
       <c r="F31" t="n">
         <v>0</v>
       </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
         <v>631</v>
       </c>
@@ -4996,11 +5050,18 @@
       <c r="K32" t="n">
         <v>661</v>
       </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
         <v>76</v>
       </c>
@@ -5016,11 +5077,23 @@
       <c r="K33" t="n">
         <v>661</v>
       </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="n">
         <v>21.75999999999999</v>
       </c>

</xml_diff>